<commit_message>
revise fitness and add iteration reports
</commit_message>
<xml_diff>
--- a/src/data/input.xlsx
+++ b/src/data/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khaibnd/eclipse-workspace/LNWG3/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khaibnd/eclipse-workspace/LNWG4/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8E540E-736C-5643-827F-A07511580F6B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4F8203-E66D-304B-A645-F90657E9828F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="4920" windowWidth="17760" windowHeight="10040" xr2:uid="{CA00F4A2-42BA-FF4B-A33E-1C1F5A5699E6}"/>
+    <workbookView xWindow="7840" yWindow="4660" windowWidth="17760" windowHeight="10040" xr2:uid="{CA00F4A2-42BA-FF4B-A33E-1C1F5A5699E6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="68">
   <si>
     <t>part</t>
   </si>
@@ -238,16 +238,20 @@
   </si>
   <si>
     <t>blo_2</t>
+  </si>
+  <si>
+    <t>work_hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,6 +264,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -332,10 +343,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -374,8 +386,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -702,7 +716,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,7 +753,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -747,7 +761,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="10">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -755,7 +769,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="10">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -763,7 +777,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="10">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -771,7 +785,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="10">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -787,7 +801,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="10">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +862,7 @@
       </c>
       <c r="C2" s="12">
         <f ca="1">TODAY()</f>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D2" s="1">
         <v>1000</v>
@@ -871,7 +885,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C9" ca="1" si="0">TODAY()</f>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D3" s="1">
         <v>1000</v>
@@ -894,7 +908,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D4" s="1">
         <v>1000</v>
@@ -919,7 +933,7 @@
       </c>
       <c r="C5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D5" s="1">
         <v>1000</v>
@@ -944,7 +958,7 @@
       </c>
       <c r="C6" s="12">
         <f ca="1">TODAY()</f>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -968,7 +982,7 @@
       </c>
       <c r="C7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -991,7 +1005,7 @@
       </c>
       <c r="C8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1016,7 +1030,7 @@
       </c>
       <c r="C9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43379</v>
+        <v>43382</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1698,7 +1712,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1729,6 +1743,9 @@
       <c r="F1" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="G1" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="L1" s="22"/>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
@@ -1754,6 +1771,9 @@
         <f t="shared" ref="F2:F12" si="1">VLOOKUP(D2,L:N,3,FALSE)</f>
         <v>0.99930555555555556</v>
       </c>
+      <c r="G2" s="24">
+        <v>24</v>
+      </c>
       <c r="L2" s="17">
         <v>1</v>
       </c>
@@ -1785,6 +1805,9 @@
         <f t="shared" si="1"/>
         <v>0.99930555555555556</v>
       </c>
+      <c r="G3" s="24">
+        <v>24</v>
+      </c>
       <c r="L3" s="17">
         <v>2</v>
       </c>
@@ -1816,6 +1839,9 @@
         <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
+      <c r="G4" s="24">
+        <v>18</v>
+      </c>
       <c r="L4" s="17">
         <v>3</v>
       </c>
@@ -1847,6 +1873,9 @@
         <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
+      <c r="G5" s="24">
+        <v>18</v>
+      </c>
       <c r="J5" s="19"/>
       <c r="L5" s="17">
         <v>4</v>
@@ -1879,6 +1908,9 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
+      <c r="G6" s="24">
+        <v>12</v>
+      </c>
       <c r="L6" s="17">
         <v>5</v>
       </c>
@@ -1910,6 +1942,9 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
+      <c r="G7" s="24">
+        <v>12</v>
+      </c>
       <c r="L7" s="17">
         <v>6</v>
       </c>
@@ -1941,6 +1976,9 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
+      <c r="G8" s="24">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1963,6 +2001,9 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
+      <c r="G9" s="24">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1985,6 +2026,9 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
+      <c r="G10" s="24">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -2007,6 +2051,9 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
+      <c r="G11" s="24">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -2028,6 +2075,9 @@
       <c r="F12" s="21">
         <f t="shared" si="1"/>
         <v>0.75</v>
+      </c>
+      <c r="G12" s="24">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revise fitness coat design
</commit_message>
<xml_diff>
--- a/src/data/input.xlsx
+++ b/src/data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khaibnd/eclipse-workspace/LNWG4/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808AD8A-027A-E64A-BB9D-2CA38C4C67EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3E262A-8050-7843-ADDE-A977919B0005}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2560" yWindow="1620" windowWidth="21560" windowHeight="13460" tabRatio="872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -820,7 +820,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>